<commit_message>
add sorting muscles by muscleGroup
</commit_message>
<xml_diff>
--- a/src/main/resources/filesCSV/Muscles.xlsx
+++ b/src/main/resources/filesCSV/Muscles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcolesnic\IdeaProjects\FitnessProj\TrainingWeb\src\main\resources\filesCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D60ED4F-4F23-4354-9029-97A596389F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFA70DF-A0AF-4D7A-9424-ECC5E51C74F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,9 +126,6 @@
     <t>Широчайшие мышцы спины</t>
   </si>
   <si>
-    <t>Ромбовидный мускул</t>
-  </si>
-  <si>
     <t>Малая круглая мышца</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>Большая ягодичная мышца</t>
+  </si>
+  <si>
+    <t>Ромбовидная мышца</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="4"/>
@@ -812,7 +812,7 @@
         <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="4"/>
@@ -836,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="4"/>
@@ -858,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="4"/>
@@ -1025,7 +1025,7 @@
         <v>19</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21">
@@ -1054,7 +1054,7 @@
         <v>20</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22">
@@ -1083,7 +1083,7 @@
         <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23">
@@ -1279,7 +1279,7 @@
     </row>
     <row r="33" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F33" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G33" s="4"/>
       <c r="J33" s="5" t="s">
@@ -1318,21 +1318,21 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F35" s="2"/>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J35" s="2"/>
       <c r="L35">
         <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N35" s="2"/>
       <c r="Q35" s="4"/>
@@ -1342,21 +1342,21 @@
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F36" s="3"/>
       <c r="H36">
         <v>2</v>
       </c>
       <c r="I36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J36" s="3"/>
       <c r="L36">
         <v>2</v>
       </c>
       <c r="M36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N36" s="3"/>
       <c r="Q36" s="4"/>
@@ -1366,21 +1366,21 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F37" s="3"/>
       <c r="H37">
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J37" s="3"/>
       <c r="L37">
         <v>3</v>
       </c>
       <c r="M37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N37" s="3"/>
       <c r="Q37" s="4"/>
@@ -1395,7 +1395,7 @@
         <v>4</v>
       </c>
       <c r="I38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J38" s="3"/>
       <c r="L38">
@@ -1415,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="I39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J39" s="3"/>
       <c r="L39">
@@ -1435,7 +1435,7 @@
         <v>6</v>
       </c>
       <c r="I40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J40" s="3"/>
       <c r="L40">
@@ -1455,7 +1455,7 @@
         <v>7</v>
       </c>
       <c r="I41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J41" s="3"/>
       <c r="L41">
@@ -1475,7 +1475,7 @@
         <v>8</v>
       </c>
       <c r="I42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J42" s="3"/>
       <c r="L42">

</xml_diff>

<commit_message>
Feature/add sort exercise by muscle groups (#6)
* add sorting muscles by muscleGroup

* add sorting exercises
</commit_message>
<xml_diff>
--- a/src/main/resources/filesCSV/Muscles.xlsx
+++ b/src/main/resources/filesCSV/Muscles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcolesnic\IdeaProjects\FitnessProj\TrainingWeb\src\main\resources\filesCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D60ED4F-4F23-4354-9029-97A596389F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFA70DF-A0AF-4D7A-9424-ECC5E51C74F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,9 +126,6 @@
     <t>Широчайшие мышцы спины</t>
   </si>
   <si>
-    <t>Ромбовидный мускул</t>
-  </si>
-  <si>
     <t>Малая круглая мышца</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>Большая ягодичная мышца</t>
+  </si>
+  <si>
+    <t>Ромбовидная мышца</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="4"/>
@@ -812,7 +812,7 @@
         <v>4</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="4"/>
@@ -836,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="4"/>
@@ -858,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="4"/>
@@ -1025,7 +1025,7 @@
         <v>19</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21">
@@ -1054,7 +1054,7 @@
         <v>20</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22">
@@ -1083,7 +1083,7 @@
         <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23">
@@ -1279,7 +1279,7 @@
     </row>
     <row r="33" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F33" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G33" s="4"/>
       <c r="J33" s="5" t="s">
@@ -1318,21 +1318,21 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F35" s="2"/>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J35" s="2"/>
       <c r="L35">
         <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N35" s="2"/>
       <c r="Q35" s="4"/>
@@ -1342,21 +1342,21 @@
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F36" s="3"/>
       <c r="H36">
         <v>2</v>
       </c>
       <c r="I36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J36" s="3"/>
       <c r="L36">
         <v>2</v>
       </c>
       <c r="M36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N36" s="3"/>
       <c r="Q36" s="4"/>
@@ -1366,21 +1366,21 @@
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F37" s="3"/>
       <c r="H37">
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J37" s="3"/>
       <c r="L37">
         <v>3</v>
       </c>
       <c r="M37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N37" s="3"/>
       <c r="Q37" s="4"/>
@@ -1395,7 +1395,7 @@
         <v>4</v>
       </c>
       <c r="I38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J38" s="3"/>
       <c r="L38">
@@ -1415,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="I39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J39" s="3"/>
       <c r="L39">
@@ -1435,7 +1435,7 @@
         <v>6</v>
       </c>
       <c r="I40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J40" s="3"/>
       <c r="L40">
@@ -1455,7 +1455,7 @@
         <v>7</v>
       </c>
       <c r="I41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J41" s="3"/>
       <c r="L41">
@@ -1475,7 +1475,7 @@
         <v>8</v>
       </c>
       <c r="I42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J42" s="3"/>
       <c r="L42">

</xml_diff>

<commit_message>
Add trainingElements and Training
</commit_message>
<xml_diff>
--- a/src/main/resources/filesCSV/Muscles.xlsx
+++ b/src/main/resources/filesCSV/Muscles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcolesnic\IdeaProjects\FitnessProj\TrainingWeb\src\main\resources\filesCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161EA647-1CC8-44CB-BC66-C066ECFEAB0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7F519C-DC17-453E-8AA0-33475684812A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="118">
   <si>
     <t>Название</t>
   </si>
@@ -468,12 +468,6 @@
     <t>двуглавая мышца бедра</t>
   </si>
   <si>
-    <t>Длинная головка прикрепляется к бугорку седалищной кости, короткая - к латеральной губе</t>
-  </si>
-  <si>
-    <t>Эта мышца помогает в выпрямлении ноги, сгибает голень и вращает ее в согнутом коленном суставе наружу.</t>
-  </si>
-  <si>
     <t>полусухожильная мышца</t>
   </si>
   <si>
@@ -486,9 +480,6 @@
     <t>полуперепончатая мышца</t>
   </si>
   <si>
-    <t>Крепится к медиальному суставному мыщелку большеберцовой кости</t>
-  </si>
-  <si>
     <t>По функциональности совпадает с полусухожильной</t>
   </si>
   <si>
@@ -626,13 +617,962 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>Двуглавая мышца бедра</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (бицепс </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>бедра</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) — длинная </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>мышца</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, проходящая по всей задней части </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>бедра</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Состоит из длинной и короткой головок. Верхним концом длинной головки крепится к седалищному бугру тазовой кости, а нижним — к берцовой кости.</t>
+    </r>
+  </si>
+  <si>
+    <t>При укреплённой голени производят разгибание туловища совместно с большой ягодичной мышцей. Когда колено согнуто, те же мышцы осуществляют вращение голени, сокращаясь по отдельности на той или другой стороне. Двуглавая мышца бедра вращает голень кнаружи</t>
+  </si>
+  <si>
+    <t>Прямая мышца бедра</t>
+  </si>
+  <si>
+    <r>
+      <t>Прямая мышца бедра (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>musculus rectus femoris</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) наиболее длинная из всех головок мышцы. Состоит из двух головок: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>прямая головка</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>caput rectum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (A04.7.02.019)) и </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>загнутая головка</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>caput reflexum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (A04.7.02.020))</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[3]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Занимает переднюю поверхность бедра. Начинается тонким сухожилием от </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>нижней передней ости</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>надвертлужной борозды</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> подвздошной кости. В самом начале прикрыта мышцей, напрягающей широкую фасцию бедра и портняжной мышцей</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[4]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Направляется вниз и переходит в узкое сухожилие, которое входит в состав общего </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>сухожилия четырёхглавой мышцы</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Достигнув большеберцовой кости сухожилие прикрепляется к </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>большеберцовой бугристости</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Ниже надколенника оно называется </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>связкой надколенника</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ligamentum patellae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Медиальная широкая мышца бедра (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>musculus vastus medialis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) занимает переднемедиальную поверхность нижней половины бедра. Мышца берёт начало от </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>медиальной губы</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>шероховатой линии</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> бедренной кости и, направляясь вниз, переходит в широкое сухожилие, которое частично вплетается в широкое сухожилие вместе с </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>прямой мышцей бедра</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, а частично прикрепляется к медиальному краю надколенника, образуя </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>медиальную поддерживающую связку надколенника</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Таким образом образующие мышцу пучки направлены косо сверху вниз и изнутри наперёд</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Медиальная широкая мышца бедра</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Разгибает голень в коленном суставе. Прямая мышца бедра, перекидывающаяся через тазобедренный сустав, принимает участие в сгибании бедра, притягивает бедренную кость к подвздошной кости, способствует удержанию </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>головки бедренной кости</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> внутри </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>вертлужной впадины</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[en]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>acetabulum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Полусухожильная мышца располагается ближе к медиальному краю задней поверхности бедра. Наружная её сторона граничит с двуглавой мышцей бедра (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Musculus biceps femoris</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), внутренняя — с полуперепончатой (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Musculus semimembranosus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>). Проксимальный отдел мышцы прикрыт большой ягодичной мышцей</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Посередине мышца часто прерывается косо идущей сухожильной перемычкой. Начинаясь от </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>седалищного бугра</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ветви седалищной кости она следует вниз, переходит в длинное сухожилие, которое обогнув медиальный надмыщелок бедра, следует к переднемедиальной поверхности большеберцовой кости, прикрепляясь к её бугристости. Часть концевых пучков сухожилия вплетается в фасцию голени</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.Сухожилие мышцы у места своего прикрепления вместе с сухожилием тонкой и портняжной мышц образует трееугольное, соединяющееся с fascia cruris сухожильное растяжение, так называемую поверхностную гусиную лапку (лат. pes anserinus superficialis)</t>
+    </r>
+  </si>
+  <si>
+    <t>Латеральная широкая мышца бедра</t>
+  </si>
+  <si>
+    <r>
+      <t>Латеральная широкая мышца бедра (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>musculus vastus lateralis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) занимает почти всю переднелатеральную поверхность бедра. Сверху она несколько прикрыта </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>мышцей, напрягающей широкую фасцию</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, а спереди — </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>прямой мышцей бедра</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Мышца начинается от большого вертела, межвертельной линии и латеральной губы шероховатой линии бедра. Направляясь вниз, мышца переходит в широкое сухожилие, которое входит в состав общего сухожилия четырёхглавой мышцы и участвует в образовании латеральной поддерживающей связки надколенника</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Портня́жная мы́шца</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Сгибает ногу в тазобедренном и коленном суставах: вращает голень внутрь, а бедро — наружу. Тем самым принимает участие в забрасывании ноги за ногу</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[3]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.Участвует в выпрямлении бедра, препятствует выворачиванию бедра внутрь во время приседаний.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Портня́жная мы́шца</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (лат. musculus sartorius) — </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>мышца</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> передней группы </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>бедра</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Является наиболее длинной мышцей человеческого организма.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Начинается от передней верхней подвздошной ости подвздошной кости. Направляется от неё косо вниз. Располагаясь на передней поверхности бедра, мышца спиралеобразно направляется вниз, переходя на его внутреннюю поверхность, а затем, обогнув сзади медиальный надмыщелок, переходит на переднемедиальную поверхность голени.Мышца переходит в плоское сухожилие, которое прикрепляется к бугристости большеберцовой кости, а некоторое число пучков вплетается в фасцию верхнего отдела голени. У места прикрепления мышцы образуются 2—3 подсухожильные сумки портняжной мышцы (лат. bursae subtendineae m. sartorii), которые отделяют сухожилие последней от сухожилий тонкой и полусухожильной мышц. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Длинная приводящая мышца</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (лат. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Musculus adductor longus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) — плоская, по форме несколько напоминает треугольник, располагается на переднемедиальной поверхности бедра.</t>
+    </r>
+  </si>
+  <si>
+    <t>Длинная приводящая мышца</t>
+  </si>
+  <si>
+    <t>Приводит бедро, принимая участие в его сгибании и вращении кнаружи.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -667,6 +1607,22 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -808,7 +1764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -829,6 +1785,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1112,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,7 +2245,7 @@
         <v>15</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="O8" s="1"/>
       <c r="Q8" s="4"/>
@@ -1296,10 +2258,10 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H9">
         <v>4</v>
@@ -1562,10 +2524,10 @@
         <v>16</v>
       </c>
       <c r="N21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="O21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="Q21" s="4"/>
     </row>
@@ -1600,10 +2562,10 @@
         <v>17</v>
       </c>
       <c r="N22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O22" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="Q22" s="4"/>
     </row>
@@ -1636,10 +2598,10 @@
         <v>18</v>
       </c>
       <c r="N23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="O23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q23" s="4"/>
     </row>
@@ -1888,23 +2850,23 @@
       <c r="I35" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="J35" t="s">
-        <v>81</v>
-      </c>
-      <c r="K35" t="s">
-        <v>82</v>
+      <c r="J35" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="L35">
         <v>1</v>
       </c>
       <c r="M35" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N35" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O35" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Q35" s="4"/>
     </row>
@@ -1925,29 +2887,29 @@
         <v>2</v>
       </c>
       <c r="I36" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="J36" t="s">
+        <v>82</v>
+      </c>
+      <c r="K36" t="s">
         <v>83</v>
-      </c>
-      <c r="J36" t="s">
-        <v>84</v>
-      </c>
-      <c r="K36" t="s">
-        <v>85</v>
       </c>
       <c r="L36">
         <v>2</v>
       </c>
       <c r="M36" t="s">
+        <v>89</v>
+      </c>
+      <c r="N36" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="O36" t="s">
         <v>92</v>
       </c>
-      <c r="N36" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="O36" t="s">
-        <v>95</v>
-      </c>
       <c r="Q36" s="4"/>
     </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:17" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D37">
         <v>3</v>
       </c>
@@ -1964,29 +2926,29 @@
         <v>3</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J37" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="K37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L37">
         <v>3</v>
       </c>
       <c r="M37" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N37" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Q37" s="4"/>
     </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:17" ht="18" x14ac:dyDescent="0.3">
       <c r="D38">
         <v>4</v>
       </c>
@@ -1996,8 +2958,15 @@
       <c r="H38">
         <v>4</v>
       </c>
-      <c r="J38" s="3"/>
-      <c r="K38" s="1"/>
+      <c r="I38" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="J38" t="s">
+        <v>105</v>
+      </c>
+      <c r="K38" t="s">
+        <v>108</v>
+      </c>
       <c r="L38">
         <v>4</v>
       </c>
@@ -2006,7 +2975,7 @@
       <c r="O38" s="13"/>
       <c r="Q38" s="4"/>
     </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:17" ht="18" x14ac:dyDescent="0.3">
       <c r="D39">
         <v>5</v>
       </c>
@@ -2016,8 +2985,12 @@
       <c r="H39">
         <v>5</v>
       </c>
-      <c r="J39" s="3"/>
-      <c r="K39" s="1"/>
+      <c r="I39" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="J39" t="s">
+        <v>106</v>
+      </c>
       <c r="L39">
         <v>5</v>
       </c>
@@ -2026,7 +2999,7 @@
       <c r="O39" s="1"/>
       <c r="Q39" s="4"/>
     </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:17" ht="18" x14ac:dyDescent="0.3">
       <c r="D40">
         <v>6</v>
       </c>
@@ -2036,7 +3009,12 @@
       <c r="H40">
         <v>6</v>
       </c>
-      <c r="J40" s="3"/>
+      <c r="I40" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="J40" t="s">
+        <v>111</v>
+      </c>
       <c r="K40" s="1"/>
       <c r="L40">
         <v>6</v>
@@ -2046,7 +3024,7 @@
       <c r="O40" s="1"/>
       <c r="Q40" s="4"/>
     </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:17" ht="16.2" x14ac:dyDescent="0.3">
       <c r="D41">
         <v>7</v>
       </c>
@@ -2056,8 +3034,15 @@
       <c r="H41">
         <v>7</v>
       </c>
-      <c r="J41" s="3"/>
-      <c r="K41" s="1"/>
+      <c r="I41" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K41" t="s">
+        <v>113</v>
+      </c>
       <c r="L41">
         <v>7</v>
       </c>
@@ -2066,7 +3051,7 @@
       <c r="O41" s="1"/>
       <c r="Q41" s="4"/>
     </row>
-    <row r="42" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D42">
         <v>8</v>
       </c>
@@ -2076,8 +3061,15 @@
       <c r="H42">
         <v>8</v>
       </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="1"/>
+      <c r="I42" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>117</v>
+      </c>
       <c r="L42">
         <v>8</v>
       </c>
@@ -2455,8 +3447,10 @@
     <hyperlink ref="M37" r:id="rId29" tooltip="Подошвенная мышца" display="http://sportwiki.to/%D0%9F%D0%BE%D0%B4%D0%BE%D1%88%D0%B2%D0%B5%D0%BD%D0%BD%D0%B0%D1%8F_%D0%BC%D1%8B%D1%88%D1%86%D0%B0" xr:uid="{EE18C17B-00D0-4BA5-8509-D8B7FC494E31}"/>
     <hyperlink ref="N37" r:id="rId30" tooltip="Подошвенная мышца" display="http://sportwiki.to/%D0%9F%D0%BE%D0%B4%D0%BE%D1%88%D0%B2%D0%B5%D0%BD%D0%BD%D0%B0%D1%8F_%D0%BC%D1%8B%D1%88%D1%86%D0%B0" xr:uid="{6C2F05B9-031A-4E53-BE3C-9427C8FFDEB9}"/>
     <hyperlink ref="N8" r:id="rId31" tooltip="Анатомия шейного отдела позвоночника" display="http://sportwiki.to/%D0%90%D0%BD%D0%B0%D1%82%D0%BE%D0%BC%D0%B8%D1%8F_%D1%88%D0%B5%D0%B9%D0%BD%D0%BE%D0%B3%D0%BE_%D0%BE%D1%82%D0%B4%D0%B5%D0%BB%D0%B0_%D0%BF%D0%BE%D0%B7%D0%B2%D0%BE%D0%BD%D0%BE%D1%87%D0%BD%D0%B8%D0%BA%D0%B0" xr:uid="{23A2B226-B0D1-4652-96C0-D7DE88E29259}"/>
+    <hyperlink ref="K35" r:id="rId32" tooltip="Большая ягодичная мышца" display="https://ru.wikipedia.org/wiki/%D0%91%D0%BE%D0%BB%D1%8C%D1%88%D0%B0%D1%8F_%D1%8F%D0%B3%D0%BE%D0%B4%D0%B8%D1%87%D0%BD%D0%B0%D1%8F_%D0%BC%D1%8B%D1%88%D1%86%D0%B0" xr:uid="{3D9C0C58-E58D-4D5D-A831-6ACCD1C4A221}"/>
+    <hyperlink ref="K42" r:id="rId33" tooltip="Бедро" display="https://ru.wikipedia.org/wiki/%D0%91%D0%B5%D0%B4%D1%80%D0%BE" xr:uid="{DEACA39C-19B0-43F6-8C2E-404CBB0A5A45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>